<commit_message>
Update code for stratum that is census. New vignette for Domain stratification by Heard.
</commit_message>
<xml_diff>
--- a/inst/extdata/SampleMooseSurveyData.xlsx
+++ b/inst/extdata/SampleMooseSurveyData.xlsx
@@ -1,24 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cschwarz/Dropbox/00-current-tasks/2020-04-30-MoosePop/SightabilityModel/SightabilityModel/inst/extdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cschwarz/Dropbox/Consulting/2020-04-30-MoosePop/SightabilityModel/SightabilityModel/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDF4DA2A-671A-7849-A9E4-9888A13B21B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3971F85-56FB-E54C-AD9E-FAE79FDDE12F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18820" yWindow="2600" windowWidth="29940" windowHeight="21480" tabRatio="925" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18820" yWindow="2600" windowWidth="29940" windowHeight="21480" tabRatio="925" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BlockData" sheetId="11" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="28" r:id="rId2"/>
-    <sheet name="BlockArea" sheetId="15" r:id="rId3"/>
-    <sheet name="Stratum" sheetId="26" r:id="rId4"/>
-    <sheet name="Stratum-DomainA" sheetId="29" r:id="rId5"/>
-    <sheet name="SightabilityModel" sheetId="27" r:id="rId6"/>
+    <sheet name="BlockArea" sheetId="15" r:id="rId2"/>
+    <sheet name="Stratum" sheetId="26" r:id="rId3"/>
+    <sheet name="Stratum-DomainA" sheetId="29" r:id="rId4"/>
+    <sheet name="SightabilityModel" sheetId="27" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BlockData!$B$2:$K$616</definedName>
@@ -735,8 +734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K616"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A591" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A127" sqref="A127:A286"/>
     </sheetView>
   </sheetViews>
@@ -13927,22 +13926,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B44B148B-B839-6A4E-B01C-088022DCAF75}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:N205"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
@@ -15283,7 +15270,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{557D1C58-6BD6-CF4E-ADC6-B1EDFFC50CF3}">
   <dimension ref="A1:D6"/>
   <sheetViews>
@@ -15351,7 +15338,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{748F7ADC-052E-894E-9908-357F935346B1}">
   <dimension ref="A1:D6"/>
   <sheetViews>
@@ -15419,7 +15406,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98E9459C-0722-EA44-BA14-FEB49BCBDF6C}">
   <dimension ref="A1:C6"/>
   <sheetViews>

</xml_diff>